<commit_message>
Imported hospital facility [OMRSE:00000063]; residential facility [OMRSE:00000191]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>facility [OMRSE:00000062]; healthcare facility [OMRSE:00000102];  emergency department facility [OMRSE:00000114];  rehabilitation facility [OMRSE:00000106]</t>
+          <t>emergency department facility [OMRSE:00000114]; hospital facility [OMRSE:00000063]; healthcare facility [OMRSE:00000102]; rehabilitation facility [OMRSE:00000106]; residential facility [OMRSE:00000191]; facility [OMRSE:00000062]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1201,34 +1201,6 @@
           <t>all</t>
         </is>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>SIO</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>http://purl.obolibrary.org/obo/sio.owl</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>entity [BFO:0000001]</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>geographic region [SIO:000414]; geolegal region [SIO:000413]; geopolitical region [SIO:000415]</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>all</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Imported hospital outpatient facility [BCIO:026015]; bisexual [BCIO:015050]; highest level of formal educational qualification achieved [BCIO:015240]; inpatient role [BCIO:015420]; outpatient role [BCIO:015425]; person experiencing homelessness [BCIO:015205]; consumption behaviour [BCIO:036061]; prescribing behaviour [BCIO:050354]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>﻿personal role [BCIO:006081]; individual human activity [BCIO:040000]; human behaviour [BCIO:042000]; highest level of formal educational qualification achieved [BCIO:015240]; personal quality [BCIO:050303]; bisexual [BCIO:015050]; population behaviour [BCIO:034000]; consumption behaviour [BCIO:036061]; personal attribute [BCIO:050300]; human age [BCIO:015015]; individual human behaviour [BCIO:036000]; personal life attribute [BCIO:050302]; inpatient role [BCIO:015420]; person experiencing homelessness [BCIO:015205]; personal disposition [BCIO:050301]; outpatient role [BCIO:015425]; human population [BCIO:041000]; process attribute [BCIO:043000]; intervention [BCIO:037000]; prescribing behaviour [BCIO:050354]</t>
+          <t>human population [BCIO:041000]; population behaviour [BCIO:034000]; ﻿personal role [BCIO:006081]; intervention [BCIO:037000]; individual human activity [BCIO:040000]; outpatient role [BCIO:015425]; highest level of formal educational qualification achieved [BCIO:015240]; human age [BCIO:015015]; person experiencing homelessness [BCIO:015205]; personal attribute [BCIO:050300]; individual human behaviour [BCIO:036000]; process attribute [BCIO:043000]; bisexual [BCIO:015050]; consumption behaviour [BCIO:036061]; hospital outpatient facility [BCIO:026015]; personal quality [BCIO:050303]; inpatient role [BCIO:015420]; personal disposition [BCIO:050301]; human behaviour [BCIO:042000]; personal life attribute [BCIO:050302]; prescribing behaviour [BCIO:050354]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>emergency department facility [OMRSE:00000114]; hospital facility [OMRSE:00000063]; healthcare facility [OMRSE:00000102]; rehabilitation facility [OMRSE:00000106]; residential facility [OMRSE:00000191]; facility [OMRSE:00000062]</t>
+          <t>facility [OMRSE:00000062]; healthcare facility [OMRSE:00000102];  emergency department facility [OMRSE:00000114];  rehabilitation facility [OMRSE:00000106]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">

</xml_diff>

<commit_message>
Imported laboratory facility [ENVO:01001406]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>human population [BCIO:041000]; population behaviour [BCIO:034000]; ﻿personal role [BCIO:006081]; intervention [BCIO:037000]; individual human activity [BCIO:040000]; outpatient role [BCIO:015425]; highest level of formal educational qualification achieved [BCIO:015240]; human age [BCIO:015015]; person experiencing homelessness [BCIO:015205]; personal attribute [BCIO:050300]; individual human behaviour [BCIO:036000]; process attribute [BCIO:043000]; bisexual [BCIO:015050]; consumption behaviour [BCIO:036061]; hospital outpatient facility [BCIO:026015]; personal quality [BCIO:050303]; inpatient role [BCIO:015420]; personal disposition [BCIO:050301]; human behaviour [BCIO:042000]; personal life attribute [BCIO:050302]; prescribing behaviour [BCIO:050354]</t>
+          <t>﻿personal role [BCIO:006081]; individual human activity [BCIO:040000]; human behaviour [BCIO:042000]; highest level of formal educational qualification achieved [BCIO:015240]; personal quality [BCIO:050303]; bisexual [BCIO:015050]; population behaviour [BCIO:034000]; consumption behaviour [BCIO:036061]; personal attribute [BCIO:050300]; human age [BCIO:015015]; individual human behaviour [BCIO:036000]; personal life attribute [BCIO:050302]; inpatient role [BCIO:015420]; person experiencing homelessness [BCIO:015205]; personal disposition [BCIO:050301]; outpatient role [BCIO:015425]; human population [BCIO:041000]; process attribute [BCIO:043000]; intervention [BCIO:037000]; prescribing behaviour [BCIO:050354]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -760,7 +760,7 @@
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>﻿human construction [ENVO:00000070];building [ENVO:00000073];shop [ENVO:00002221];environmental material [ENVO:00010483];aerosol [ENVO:00010505];environmental system [ENVO:01000254];environmental disposition [ENVO:01000452];fire [ENVO:01000786];smoke [ENVO:01000838];commercial building [ENVO:01001222];construction [ENVO:01001813]</t>
+          <t>fire [ENVO:01000786]; ﻿human construction [ENVO:00000070]; building [ENVO:00000073]; environmental disposition [ENVO:01000452]; aerosol [ENVO:00010505]; construction [ENVO:01001813]; smoke [ENVO:01000838]; environmental system [ENVO:01000254]; laboratory facility [ENVO:01001406]; shop [ENVO:00002221]; environmental material [ENVO:00010483]; commercial building [ENVO:01001222]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">

</xml_diff>

<commit_message>
Imported adverse treatment outcome [PATO:0000011]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -760,7 +760,7 @@
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>fire [ENVO:01000786]; ﻿human construction [ENVO:00000070]; building [ENVO:00000073]; environmental disposition [ENVO:01000452]; aerosol [ENVO:00010505]; construction [ENVO:01001813]; smoke [ENVO:01000838]; environmental system [ENVO:01000254]; laboratory facility [ENVO:01001406]; shop [ENVO:00002221]; environmental material [ENVO:00010483]; commercial building [ENVO:01001222]</t>
+          <t>﻿human construction [ENVO:00000070];building [ENVO:00000073];shop [ENVO:00002221];environmental material [ENVO:00010483];aerosol [ENVO:00010505];environmental system [ENVO:01000254];environmental disposition [ENVO:01000452];fire [ENVO:01000786];smoke [ENVO:01000838];commercial building [ENVO:01001222];construction [ENVO:01001813]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>physical quality [PATO:0001018]; concentration [PATO:0000033]</t>
+          <t>adverse treatment outcome [PATO:0000011]; physical quality [PATO:0001018]; concentration [PATO:0000033]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">

</xml_diff>

<commit_message>
Imported agitation [NCIT:C79530]; thalamus [NCIT:C12459]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>adverse treatment outcome [PATO:0000011]; physical quality [PATO:0001018]; concentration [PATO:0000033]</t>
+          <t>physical quality [PATO:0001018]; concentration [PATO:0000033]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1201,6 +1201,34 @@
           <t>all</t>
         </is>
       </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>NCIT</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>http://purl.obolibrary.org/obo/ncit.owl</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>entity [BFO:0000001]</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>agitation [NCIT:C79530]; thalamus [NCIT:C12459]</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Imported aortic stiffness [HP:0030965]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -1205,12 +1205,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>NCIT</t>
+          <t>HP</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/ncit.owl</t>
+          <t>http://purl.obolibrary.org/obo/hp.owl</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>agitation [NCIT:C79530]; thalamus [NCIT:C12459]</t>
+          <t>aortic stiffness [HP:0030965]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">

</xml_diff>

<commit_message>
Imported cotinine [CHEBI:68641]; acetaldehyde [CHEBI:15343]; acrolein [CHEBI:15368]; acrylonitrile [CHEBI:28217]; metabolite [CHEBI:25212]; 4-(methylnitrosamino)-1-(3-pyridyl)-1-butanol [CHEBI:82569]; acetylcysteine [CHEBI:22198]; aripiprazole [CHEBI:31236]; methanol [CHEBI:17790]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -1205,12 +1205,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>CHEBI</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/hp.owl</t>
+          <t>http://purl.obolibrary.org/obo/chebi.owl</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>aortic stiffness [HP:0030965]</t>
+          <t>cotinine [CHEBI:68641]; acetaldehyde [CHEBI:15343]; acrolein [CHEBI:15368]; acrylonitrile [CHEBI:28217]; metabolite [CHEBI:25212]; 4-(methylnitrosamino)-1-(3-pyridyl)-1-butanol [CHEBI:82569]; acetylcysteine [CHEBI:22198]; aripiprazole [CHEBI:31236]; methanol [CHEBI:17790]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">

</xml_diff>

<commit_message>
Imported patient role [OBI:0000093]; protocol [OBI:0000272]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
@@ -950,7 +950,7 @@
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>protocol [OBI:0000272]; dose [OBI:0000984]; ﻿extract [OBI:0000423]; organisation [OBI:0000245]; planned process [OBI:0000011]</t>
+          <t>planned process [OBI:0000011]; patient role [OBI:0000093]; dose [OBI:0000984]; organisation [OBI:0000245]; protocol [OBI:0000272]; ﻿extract [OBI:0000423]</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1201,34 +1201,6 @@
           <t>all</t>
         </is>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>UBERON</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>http://purl.obolibrary.org/obo/uberon.owl</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>entity [BFO:0000001]</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>death [UBERON:0035944]</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>all</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Imported substance-induced anxiety disorder [ADDICTO:0001039]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
@@ -950,7 +950,7 @@
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>planned process [OBI:0000011]; patient role [OBI:0000093]; dose [OBI:0000984]; organisation [OBI:0000245]; protocol [OBI:0000272]; ﻿extract [OBI:0000423]</t>
+          <t>protocol [OBI:0000272]; dose [OBI:0000984]; ﻿extract [OBI:0000423]; organisation [OBI:0000245]; planned process [OBI:0000011]</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1201,6 +1201,34 @@
           <t>all</t>
         </is>
       </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ADDICTO</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>http://purl.obolibrary.org/obo/addicto.owl</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>entity [BFO:0000001]</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>substance-induced anxiety disorder [ADDICTO:0001039]</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Imported unemployed status [SDGIO:00010026]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -1205,12 +1205,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ADDICTO</t>
+          <t>SDGIO</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>http://purl.obolibrary.org/obo/addicto.owl</t>
+          <t>http://purl.obolibrary.org/obo/sdgio.owl</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>substance-induced anxiety disorder [ADDICTO:0001039]</t>
+          <t>unemployed status [SDGIO:00010026]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">

</xml_diff>

<commit_message>
Imported treatment satisfaction [OGMS:0000090]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
@@ -977,7 +977,7 @@
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>injury [OGMS:0000102];﻿disease [OGMS:0000031]</t>
+          <t>injury [OGMS:0000102]; treatment satisfaction [OGMS:0000090]; ﻿disease [OGMS:0000031]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1201,34 +1201,6 @@
           <t>all</t>
         </is>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>SDGIO</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>http://purl.obolibrary.org/obo/sdgio.owl</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>entity [BFO:0000001]</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>unemployed status [SDGIO:00010026]</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>all</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Imported advocacy organisation [GSSO:005379]; health organisation [GSSO:007328]; human rights organisation [GSSO:003501]; non-profit organisation [GSSO:004615]; money [GSSO:010609]
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
@@ -977,7 +977,7 @@
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>injury [OGMS:0000102]; treatment satisfaction [OGMS:0000090]; ﻿disease [OGMS:0000031]</t>
+          <t>injury [OGMS:0000102];﻿disease [OGMS:0000031]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1201,6 +1201,34 @@
           <t>all</t>
         </is>
       </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>GSSO</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>http://purl.obolibrary.org/obo/gsso.owl</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>entity [BFO:0000001]</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>advocacy organisation [GSSO:005379]; health organisation [GSSO:007328]; human rights organisation [GSSO:003501]; non-profit organisation [GSSO:004615]; money [GSSO:010609]</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reomve hospital outpatient facility [BCIO:026015]; due to weird placement in BCIO
</commit_message>
<xml_diff>
--- a/imports/External_Imports.xlsx
+++ b/imports/External_Imports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgehrk/development/addiction-ontology/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0386E96-4427-D94E-9F05-C0240E2B70ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83B24F7-708A-C349-B0B7-36FC25EBB6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1440" windowWidth="28180" windowHeight="14040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,10 +313,10 @@
     <t>Amphetamine [CHEBI:2679];Baclofen [CHEBI:2972];Benzodiazepine [CHEBI:22720];Buprenorphine [CHEBI:3216];Bupropion [CHEBI:3219];Caffeine [CHEBI:27732];Cannabinoid [CHEBI:67194];Chemical substance [CHEBI:59999];Cocaine [CHEBI:27958];Codeine [CHEBI:16714];Ethanol [CHEBI:16236];Fentanyl [CHEBI:119915];Formaldehyde [CHEBI:16842];Gabapentin [CHEBI:42797];Heroin [CHEBI:27808];Methadone [CHEBI:6807];Methadrone  [CHEBI:59331];Methamphetamine [CHEBI:6809];Naloxone [CHEBI:7459];Nicotine [CHEBI:18723];4-(N-nitrosomethylamino)-1-(3-pyridyl)butan-1-one [CHEBI:32692];Synthetic cannabinoid [CHEBI:67201];Delta(9)-tetrahydrocannabinol [CHEBI:66964];Varenicline [CHEBI:84500];nitrosamine [CHEBI:35803]; Atomoxetine [CHEBI:127342];naphthalene [CHEBI:16482];propanal [CHEBI:17153];carbon monoxide [CHEBI:17245]; nicotine [CHEBI:18723]; carbonyl compound [CHEBI:36586]; elemental cadmium [CHEBI:37249]; pyrene [CHEBI:39106]; cytisine [CHEBI:4055]; crotonaldehyde [CHEBI:41607]; diazepam [CHEBI:49575]; hydrocodone [CHEBI:5779]; cannabidiol [CHEBI:69478]; oxycodone [CHEBI:7852]; rimonabant [CHEBI:34967]; MDMA [CHEBI:1391]; naltrexone [CHEBI:7465];  acetylcysteine [CHEBI:22198]; aripiprazole [CHEBI:31236]; 4-(methylnitrosamino)-1-(3-pyridyl)-1-butanol [CHEBI:82569]; cotinine [CHEBI:68641]; methanol [CHEBI:17790]</t>
   </si>
   <si>
-    <t>outpatient role [BCIO:015080]; intervention [BCIO:037000]; personal life attribute [BCIO:050302]; human population [BCIO:041000]; subjective want [BCIO:050317]; consumption behaviour [BCIO:036061];  human age [BCIO:015015]; individual human behaviour [BCIO:036000]; highest level of formal educational qualification achieved [BCIO:015243]; homeless person [BCIO:015036]; ﻿personal role [BCIO:006081]; inpatient role [BCIO:015079]; individual human activity [BCIO:040000]; personal disposition [BCIO:050301]; personal attribute [BCIO:050300]; pleasure associated with a behaviour [BCIO:006159]; hospital outpatient facility [BCIO:026015]; personal quality [BCIO:050303]; prescribing behaviour [BCIO:050354]; population behaviour [BCIO:034000]; human behaviour [BCIO:042000]; bisexual [BCIO:015005]; within-country location [BCIO:026002]; e-cigarette use [BCIO:050377]; bodily process [OGMS:0000060]; object-using behaviour [BCIO:036027]</t>
-  </si>
-  <si>
     <t>https://ftp.ebi.ac.uk/pub/databases/chebi/ontology/chebi_lite.owl</t>
+  </si>
+  <si>
+    <t>outpatient role [BCIO:015080]; intervention [BCIO:037000]; personal life attribute [BCIO:050302]; human population [BCIO:041000]; subjective want [BCIO:050317]; consumption behaviour [BCIO:036061];  human age [BCIO:015015]; individual human behaviour [BCIO:036000]; highest level of formal educational qualification achieved [BCIO:015243]; homeless person [BCIO:015036]; ﻿personal role [BCIO:006081]; inpatient role [BCIO:015079]; individual human activity [BCIO:040000]; personal disposition [BCIO:050301]; personal attribute [BCIO:050300]; pleasure associated with a behaviour [BCIO:006159]; personal quality [BCIO:050303]; prescribing behaviour [BCIO:050354]; population behaviour [BCIO:034000]; human behaviour [BCIO:042000]; bisexual [BCIO:015005]; within-country location [BCIO:026002]; e-cigarette use [BCIO:050377]; bodily process [OGMS:0000060]; object-using behaviour [BCIO:036027]</t>
   </si>
 </sst>
 </file>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -767,7 +767,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -784,7 +784,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -802,7 +802,7 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>

</xml_diff>